<commit_message>
updated summary of results
</commit_message>
<xml_diff>
--- a/data/summary_of_results.xlsx
+++ b/data/summary_of_results.xlsx
@@ -10,6 +10,7 @@
   <sheets>
     <sheet name="macro" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="sector" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="financial ratios" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="73">
   <si>
     <t xml:space="preserve">Descriptive statistics</t>
   </si>
@@ -198,17 +199,60 @@
   </si>
   <si>
     <t xml:space="preserve">Lag: +ve means the exog variable is leading wrt. HK50 (endog var)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coefficients of determination</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Financial ratio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Decision tree (train)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Decision tree (test)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gradient boost (train)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gradient boost (test)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enterprise value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Free cash flow</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EBITDA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Revenue</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Return on equity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gross profit margin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Quick ratio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Debt to equity ratio</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
+  <numFmts count="5">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0.00%"/>
     <numFmt numFmtId="166" formatCode="0.00"/>
     <numFmt numFmtId="167" formatCode="0.000000"/>
+    <numFmt numFmtId="168" formatCode="0.000"/>
   </numFmts>
   <fonts count="6">
     <font>
@@ -286,7 +330,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -315,6 +359,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -334,8 +382,8 @@
   </sheetPr>
   <dimension ref="B4:M131"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A118" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I135" activeCellId="0" sqref="I135"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2179,7 +2227,7 @@
   </sheetPr>
   <dimension ref="B4:J82"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F69" activeCellId="0" sqref="F69"/>
     </sheetView>
   </sheetViews>
@@ -3417,4 +3465,193 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="B5:F14"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E14" activeCellId="0" sqref="E14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="19.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="18.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="19.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="18.88"/>
+  </cols>
+  <sheetData>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B5" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B6" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="E6" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="F6" s="0" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B7" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="C7" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="D7" s="7" t="n">
+        <v>-2.58198612156547</v>
+      </c>
+      <c r="E7" s="7" t="n">
+        <v>0.999999995658277</v>
+      </c>
+      <c r="F7" s="7" t="n">
+        <v>-5.16351442656913</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B8" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="C8" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="D8" s="7" t="n">
+        <v>-5.05831024318142</v>
+      </c>
+      <c r="E8" s="7" t="n">
+        <v>0.999999994794889</v>
+      </c>
+      <c r="F8" s="7" t="n">
+        <v>-7.7442853512372</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B9" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="C9" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="D9" s="7" t="n">
+        <v>-8.47714095853272</v>
+      </c>
+      <c r="E9" s="7" t="n">
+        <v>0.999999896606301</v>
+      </c>
+      <c r="F9" s="7" t="n">
+        <v>-9.07728458445717</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B10" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="C10" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="D10" s="7" t="n">
+        <v>-6.64862911206342</v>
+      </c>
+      <c r="E10" s="7" t="n">
+        <v>0.999999993985728</v>
+      </c>
+      <c r="F10" s="7" t="n">
+        <v>-5.56904110699226</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B11" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="C11" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="D11" s="7" t="n">
+        <v>-6.64862911206342</v>
+      </c>
+      <c r="E11" s="7" t="n">
+        <v>0.999999996845121</v>
+      </c>
+      <c r="F11" s="7" t="n">
+        <v>-4.43375034207515</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B12" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="C12" s="7" t="n">
+        <v>0.65048829487508</v>
+      </c>
+      <c r="D12" s="7" t="n">
+        <v>-8.31246456204073</v>
+      </c>
+      <c r="E12" s="7" t="n">
+        <v>0.422532456113729</v>
+      </c>
+      <c r="F12" s="7" t="n">
+        <v>-4.96361618177758</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B13" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="C13" s="7" t="n">
+        <v>0.611219829794956</v>
+      </c>
+      <c r="D13" s="7" t="n">
+        <v>-6.64862911206342</v>
+      </c>
+      <c r="E13" s="7" t="n">
+        <v>0.292273915800679</v>
+      </c>
+      <c r="F13" s="7" t="n">
+        <v>-5.16208651074748</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B14" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="C14" s="7" t="n">
+        <v>0.611219829794956</v>
+      </c>
+      <c r="D14" s="7" t="n">
+        <v>-6.64862911206342</v>
+      </c>
+      <c r="E14" s="7" t="n">
+        <v>0.293000182550571</v>
+      </c>
+      <c r="F14" s="7" t="n">
+        <v>-9.32353157453062</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
added ridge regression results for macroeconomic indicators
</commit_message>
<xml_diff>
--- a/data/summary_of_results.xlsx
+++ b/data/summary_of_results.xlsx
@@ -5,12 +5,13 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="macro" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="sector" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="financial ratios" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="macro_ridge" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="381" uniqueCount="91">
   <si>
     <t xml:space="preserve">Descriptive statistics</t>
   </si>
@@ -219,6 +220,12 @@
     <t xml:space="preserve">Gradient boost (test)</t>
   </si>
   <si>
+    <t xml:space="preserve">SVM (train)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SVM (test)</t>
+  </si>
+  <si>
     <t xml:space="preserve">Enterprise value</t>
   </si>
   <si>
@@ -241,6 +248,54 @@
   </si>
   <si>
     <t xml:space="preserve">Debt to equity ratio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Indicator</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lag period</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ridge coefficient value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">USDHKD % change</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coincident</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AUDCNY % change</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Leading (5 days)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AUDUSD % change</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Leading (20 days)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CNYHKD % change</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DXY % change</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HKDAUD % change</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HKDEUR % change</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lagging (20 days)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coincident </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SPY % change</t>
   </si>
 </sst>
 </file>
@@ -254,11 +309,12 @@
     <numFmt numFmtId="167" formatCode="0.000000"/>
     <numFmt numFmtId="168" formatCode="0.000"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -280,9 +336,16 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <i val="true"/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -330,7 +393,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -363,6 +426,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -382,11 +449,11 @@
   </sheetPr>
   <dimension ref="B4:M131"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A115" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="23.81"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="23.22"/>
@@ -2227,14 +2294,14 @@
   </sheetPr>
   <dimension ref="B4:J82"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F69" activeCellId="0" sqref="F69"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="14.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="14.81"/>
   </cols>
   <sheetData>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3459,7 +3526,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -3472,13 +3539,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B5:F14"/>
+  <dimension ref="B5:H14"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E14" activeCellId="0" sqref="E14"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B19" activeCellId="0" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.36"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="19.18"/>
@@ -3508,10 +3575,16 @@
       <c r="F6" s="0" t="s">
         <v>64</v>
       </c>
+      <c r="G6" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="H6" s="0" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="0" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="C7" s="7" t="n">
         <v>1</v>
@@ -3525,10 +3598,16 @@
       <c r="F7" s="7" t="n">
         <v>-5.16351442656913</v>
       </c>
+      <c r="G7" s="7" t="n">
+        <v>0.611219829794956</v>
+      </c>
+      <c r="H7" s="7" t="n">
+        <v>-6.64862911206342</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="0" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="C8" s="7" t="n">
         <v>1</v>
@@ -3542,10 +3621,16 @@
       <c r="F8" s="7" t="n">
         <v>-7.7442853512372</v>
       </c>
+      <c r="G8" s="7" t="n">
+        <v>0.611219829794956</v>
+      </c>
+      <c r="H8" s="7" t="n">
+        <v>-6.64862911206342</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="0" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="C9" s="7" t="n">
         <v>1</v>
@@ -3559,10 +3644,16 @@
       <c r="F9" s="7" t="n">
         <v>-9.07728458445717</v>
       </c>
+      <c r="G9" s="7" t="n">
+        <v>0.611219829794956</v>
+      </c>
+      <c r="H9" s="7" t="n">
+        <v>-6.64862911206342</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="0" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="C10" s="7" t="n">
         <v>1</v>
@@ -3576,10 +3667,16 @@
       <c r="F10" s="7" t="n">
         <v>-5.56904110699226</v>
       </c>
+      <c r="G10" s="7" t="n">
+        <v>0.611219829794956</v>
+      </c>
+      <c r="H10" s="7" t="n">
+        <v>-6.64862911206342</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="0" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="C11" s="7" t="n">
         <v>1</v>
@@ -3593,10 +3690,16 @@
       <c r="F11" s="7" t="n">
         <v>-4.43375034207515</v>
       </c>
+      <c r="G11" s="7" t="n">
+        <v>0.611219829794956</v>
+      </c>
+      <c r="H11" s="7" t="n">
+        <v>-6.64862911206342</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="0" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C12" s="7" t="n">
         <v>0.65048829487508</v>
@@ -3610,10 +3713,16 @@
       <c r="F12" s="7" t="n">
         <v>-4.96361618177758</v>
       </c>
+      <c r="G12" s="7" t="n">
+        <v>0.611219829794956</v>
+      </c>
+      <c r="H12" s="7" t="n">
+        <v>-6.64862911206342</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="0" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="C13" s="7" t="n">
         <v>0.611219829794956</v>
@@ -3627,10 +3736,16 @@
       <c r="F13" s="7" t="n">
         <v>-5.16208651074748</v>
       </c>
+      <c r="G13" s="7" t="n">
+        <v>0.611219829794956</v>
+      </c>
+      <c r="H13" s="7" t="n">
+        <v>-6.64862911206342</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="0" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="C14" s="7" t="n">
         <v>0.611219829794956</v>
@@ -3643,12 +3758,179 @@
       </c>
       <c r="F14" s="7" t="n">
         <v>-9.32353157453062</v>
+      </c>
+      <c r="G14" s="7" t="n">
+        <v>0.611219829794956</v>
+      </c>
+      <c r="H14" s="7" t="n">
+        <v>-6.64862911206342</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="B4:D15"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E5" activeCellId="0" sqref="E5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="22.26"/>
+  </cols>
+  <sheetData>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B4" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B5" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <v>-0.153</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B6" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="D6" s="0" t="n">
+        <v>0.182</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B7" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="D7" s="0" t="n">
+        <v>0.169</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B8" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="D8" s="0" t="n">
+        <v>-0.192</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B9" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="D9" s="0" t="n">
+        <v>0.144</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B10" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="D10" s="0" t="n">
+        <v>0.186</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B11" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="D11" s="0" t="n">
+        <v>-0.207</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B12" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="D12" s="0" t="n">
+        <v>-0.063</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B13" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="C13" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="D13" s="0" t="n">
+        <v>0.111</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B14" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="D14" s="0" t="n">
+        <v>-0.607</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B15" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="C15" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="D15" s="0" t="n">
+        <v>0.106</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>

<commit_message>
final before second submit
</commit_message>
<xml_diff>
--- a/data/summary_of_results.xlsx
+++ b/data/summary_of_results.xlsx
@@ -309,7 +309,7 @@
     <numFmt numFmtId="167" formatCode="0.000000"/>
     <numFmt numFmtId="168" formatCode="0.000"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -344,11 +344,6 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -393,7 +388,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -426,10 +421,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -453,7 +444,7 @@
       <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="23.81"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="23.22"/>
@@ -2298,7 +2289,7 @@
       <selection pane="topLeft" activeCell="F69" activeCellId="0" sqref="F69"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.18"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="14.81"/>
@@ -3545,7 +3536,7 @@
       <selection pane="topLeft" activeCell="B19" activeCellId="0" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.36"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="19.18"/>
@@ -3785,14 +3776,14 @@
   <dimension ref="B4:D15"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D15" activeCellId="0" sqref="D15"/>
+      <selection pane="topLeft" activeCell="F24" activeCellId="0" sqref="F24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.68"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="22.26"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="22.27"/>
   </cols>
   <sheetData>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3818,7 +3809,7 @@
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="5" t="s">
         <v>80</v>
       </c>
       <c r="C6" s="0" t="s">

</xml_diff>